<commit_message>
Fixed incorrect coordinates discovered by Brock
</commit_message>
<xml_diff>
--- a/data-raw/Baystudy/Bay Study_Station Coordinates for Distribution_2018.xlsx
+++ b/data-raw/Baystudy/Bay Study_Station Coordinates for Distribution_2018.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbashevkin\Documents\LTMRdata\data-raw\Baystudy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C59DF2BD-1508-4A6A-B0C7-A74589215D74}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E00122A5-326B-4CD9-8B0F-CF5482528A81}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8235" yWindow="5730" windowWidth="10320" windowHeight="13545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Updated 2018" sheetId="1" r:id="rId1"/>
@@ -273,9 +273,6 @@
     <t>38° 06.330</t>
   </si>
   <si>
-    <t>-122° 43.020</t>
-  </si>
-  <si>
     <t>38° 06.252</t>
   </si>
   <si>
@@ -517,15 +514,15 @@
   </si>
   <si>
     <t>Longitude</t>
+  </si>
+  <si>
+    <t>-121° 43.020</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0.000"/>
-  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -620,7 +617,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -632,20 +629,23 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -929,30 +929,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.28515625" style="1" customWidth="1"/>
     <col min="2" max="2" width="16.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="18.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" style="10" customWidth="1"/>
     <col min="4" max="4" width="51.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="C1" s="8" t="s">
         <v>161</v>
       </c>
-      <c r="C1" s="8" t="s">
-        <v>162</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>93</v>
+      <c r="D1" s="5" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -962,11 +962,11 @@
       <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -976,11 +976,11 @@
       <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -990,11 +990,11 @@
       <c r="B4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -1004,11 +1004,11 @@
       <c r="B5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -1018,11 +1018,11 @@
       <c r="B6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -1032,11 +1032,11 @@
       <c r="B7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="4" t="s">
         <v>12</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -1046,11 +1046,11 @@
       <c r="B8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="4" t="s">
         <v>14</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -1060,11 +1060,11 @@
       <c r="B9" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="4" t="s">
         <v>16</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -1074,11 +1074,11 @@
       <c r="B10" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="4" t="s">
         <v>18</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -1088,11 +1088,11 @@
       <c r="B11" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="4" t="s">
         <v>20</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -1102,11 +1102,11 @@
       <c r="B12" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="4" t="s">
         <v>22</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -1116,39 +1116,39 @@
       <c r="B13" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="4" t="s">
         <v>24</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>154</v>
+        <v>151</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>153</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -1158,11 +1158,11 @@
       <c r="B16" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C16" s="4" t="s">
         <v>26</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -1172,11 +1172,11 @@
       <c r="B17" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C17" s="4" t="s">
         <v>28</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -1186,11 +1186,11 @@
       <c r="B18" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C18" s="4" t="s">
         <v>30</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -1200,11 +1200,11 @@
       <c r="B19" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C19" s="4" t="s">
         <v>32</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -1214,11 +1214,11 @@
       <c r="B20" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C20" s="4" t="s">
         <v>34</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -1228,11 +1228,11 @@
       <c r="B21" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C21" s="4" t="s">
         <v>36</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -1242,11 +1242,11 @@
       <c r="B22" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C22" s="4" t="s">
         <v>38</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -1256,11 +1256,11 @@
       <c r="B23" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C23" s="4" t="s">
         <v>40</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -1270,11 +1270,11 @@
       <c r="B24" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="C24" s="4" t="s">
         <v>42</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -1284,11 +1284,11 @@
       <c r="B25" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="C25" s="4" t="s">
         <v>44</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -1298,11 +1298,11 @@
       <c r="B26" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="C26" s="4" t="s">
         <v>46</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -1312,11 +1312,11 @@
       <c r="B27" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="C27" s="4" t="s">
         <v>48</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -1326,11 +1326,11 @@
       <c r="B28" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="C28" s="4" t="s">
         <v>50</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -1340,11 +1340,11 @@
       <c r="B29" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="C29" s="4" t="s">
         <v>52</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -1354,11 +1354,11 @@
       <c r="B30" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="C30" s="4" t="s">
         <v>54</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -1368,11 +1368,11 @@
       <c r="B31" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="C31" s="4" t="s">
         <v>32</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -1382,11 +1382,11 @@
       <c r="B32" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="C32" s="4" t="s">
         <v>57</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -1396,11 +1396,11 @@
       <c r="B33" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C33" s="2" t="s">
+      <c r="C33" s="4" t="s">
         <v>59</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -1410,11 +1410,11 @@
       <c r="B34" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C34" s="2" t="s">
+      <c r="C34" s="4" t="s">
         <v>61</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -1424,11 +1424,11 @@
       <c r="B35" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C35" s="2" t="s">
+      <c r="C35" s="4" t="s">
         <v>63</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -1438,11 +1438,11 @@
       <c r="B36" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="C36" s="2" t="s">
+      <c r="C36" s="4" t="s">
         <v>65</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -1452,11 +1452,11 @@
       <c r="B37" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C37" s="2" t="s">
+      <c r="C37" s="4" t="s">
         <v>67</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -1466,11 +1466,11 @@
       <c r="B38" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="C38" s="2" t="s">
+      <c r="C38" s="4" t="s">
         <v>69</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -1480,11 +1480,11 @@
       <c r="B39" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C39" s="2" t="s">
+      <c r="C39" s="4" t="s">
         <v>71</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -1494,11 +1494,11 @@
       <c r="B40" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="C40" s="2" t="s">
+      <c r="C40" s="4" t="s">
         <v>73</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -1508,11 +1508,11 @@
       <c r="B41" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="C41" s="2" t="s">
+      <c r="C41" s="4" t="s">
         <v>75</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -1522,11 +1522,11 @@
       <c r="B42" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="C42" s="2" t="s">
+      <c r="C42" s="4" t="s">
         <v>77</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -1537,10 +1537,10 @@
         <v>78</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -1551,10 +1551,10 @@
         <v>79</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -1564,11 +1564,11 @@
       <c r="B45" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="C45" s="2" t="s">
-        <v>81</v>
+      <c r="C45" s="4" t="s">
+        <v>162</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -1576,13 +1576,13 @@
         <v>752</v>
       </c>
       <c r="B46" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C46" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="C46" s="2" t="s">
-        <v>83</v>
-      </c>
       <c r="D46" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -1590,13 +1590,13 @@
         <v>760</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -1604,13 +1604,13 @@
         <v>761</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -1618,13 +1618,13 @@
         <v>762</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -1632,13 +1632,13 @@
         <v>837</v>
       </c>
       <c r="B50" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C50" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="C50" s="2" t="s">
-        <v>85</v>
-      </c>
       <c r="D50" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -1646,13 +1646,13 @@
         <v>853</v>
       </c>
       <c r="B51" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C51" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="C51" s="2" t="s">
-        <v>87</v>
-      </c>
       <c r="D51" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -1660,13 +1660,13 @@
         <v>863</v>
       </c>
       <c r="B52" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C52" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="C52" s="2" t="s">
-        <v>89</v>
-      </c>
       <c r="D52" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -1674,13 +1674,13 @@
         <v>864</v>
       </c>
       <c r="B53" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C53" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="C53" s="2" t="s">
-        <v>91</v>
-      </c>
       <c r="D53" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -1688,13 +1688,13 @@
         <v>865</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="C54" s="5" t="s">
-        <v>149</v>
+        <v>91</v>
+      </c>
+      <c r="C54" s="9" t="s">
+        <v>148</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
   </sheetData>

</xml_diff>